<commit_message>
Hoan thanh chuc nang nhap be
</commit_message>
<xml_diff>
--- a/20230904.xlsx
+++ b/20230904.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,16 +441,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Bò nằm viện</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>380</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>